<commit_message>
Updated Matriz de Riesgo
</commit_message>
<xml_diff>
--- a/Fase 1/Evidencias Proyecto/MATRIZ DE RIESGO.xlsx
+++ b/Fase 1/Evidencias Proyecto/MATRIZ DE RIESGO.xlsx
@@ -6,82 +6,145 @@
     <sheet state="visible" name="Hoja1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Hoja1!$B$7:$H$17</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Hoja1!$B$8:$H$19</definedName>
   </definedNames>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="JXeU+x/W91qcpf95pURmwurSbXoVzRoLDrX9M6SXmhI="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="/3xn+0zHcDucgwTFmd9Po6MR7MddufYpThVft8D38tw="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
   <si>
     <t>MATRIZ DE RIESGO</t>
   </si>
   <si>
+    <t>ALTO</t>
+  </si>
+  <si>
+    <t>3,8,9,14</t>
+  </si>
+  <si>
+    <t>MEDIO</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>2,4,5,6,11</t>
+  </si>
+  <si>
+    <t>BAJO</t>
+  </si>
+  <si>
+    <t>7,12</t>
+  </si>
+  <si>
+    <t>RIESGOS</t>
+  </si>
+  <si>
+    <t>PROBABILIDAD</t>
+  </si>
+  <si>
+    <t>IMPACTO</t>
+  </si>
+  <si>
+    <t>1.	Error en la autenticación con Amazon Cognito</t>
+  </si>
+  <si>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t>HIGH</t>
+  </si>
+  <si>
+    <t>Validar flujos con pruebas unitarias y manejo de errores; fallback visual.</t>
+  </si>
+  <si>
+    <t>2.	Fallo en la geolocalización</t>
+  </si>
+  <si>
     <t>MEDIUM</t>
   </si>
   <si>
-    <t>HIGH</t>
-  </si>
-  <si>
-    <t>CRITICAL</t>
-  </si>
-  <si>
-    <t>MEDIUM LOW</t>
-  </si>
-  <si>
-    <t>LOW</t>
-  </si>
-  <si>
-    <t>RIESGOS</t>
-  </si>
-  <si>
-    <t>PROBABILIDAD</t>
-  </si>
-  <si>
-    <t>IMPACTO</t>
-  </si>
-  <si>
-    <t>1.	Error en la autenticación con Amazon Cognito</t>
-  </si>
-  <si>
-    <t>2.	Fallo en la geolocalización</t>
+    <t>Manejar denegación de permisos con mensajes claros y opción de ingreso manual.</t>
   </si>
   <si>
     <t>3.	Problemas con la API de geolocalización (Google Maps / Mapbox</t>
   </si>
   <si>
+    <t>Implementar manejo de errores + servicio alternativo configurado.</t>
+  </si>
+  <si>
     <t>4.	Fallo en la comunicación entre frontend y backend</t>
   </si>
   <si>
+    <t>Uso de logs, pruebas integradas y manejo de timeouts con reintentos.</t>
+  </si>
+  <si>
     <t>5.	Error en la verificación de coberturas con aseguradoras</t>
   </si>
   <si>
+    <t>Simulación de API en desarrollo; validación previa de estructura de respuesta.</t>
+  </si>
+  <si>
     <t>6.	Fallo en el registro manual de usuarios</t>
   </si>
   <si>
+    <t>Validaciones en frontend + backend, mensajes de error claros.</t>
+  </si>
+  <si>
     <t>7.	Problema al subir imágenes a Amazon S3</t>
   </si>
   <si>
     <t>8.	Problema en la lógica de negocio de AWS Lambda</t>
   </si>
   <si>
+    <t>Pruebas unitarias + logging detallado + revisión de flujos antes de que salga a producción.</t>
+  </si>
+  <si>
     <t>9.	Fallo en el manejo de solicitudes de asistencia</t>
   </si>
   <si>
-    <t>10.	Fallo en la visualización del estado en tiempo real de la solicitud de asistencia</t>
+    <t>Validaciones por etapas y backup de datos temporales en base de datos.</t>
+  </si>
+  <si>
+    <t>10.        Tiempo Limitado</t>
+  </si>
+  <si>
+    <t>Planificación realista con priorización de funcionalidades clave.</t>
+  </si>
+  <si>
+    <t>11.      Integración de Apis con aseguradoras</t>
+  </si>
+  <si>
+    <t>Pruebas anticipadas con entornos sandbox y documentación clara.</t>
+  </si>
+  <si>
+    <t>12.       Pruebas en escenarios reales (QA)</t>
+  </si>
+  <si>
+    <t>13.       Carga académica y responsibilidades externas</t>
+  </si>
+  <si>
+    <t>Gestión de tiempos con calendario y bloques de trabajo definidos.</t>
+  </si>
+  <si>
+    <t>14.       Disponibilidad de servidores para el backend</t>
+  </si>
+  <si>
+    <t>Uso de infraestructura AWS confiable con monitoreo y escalabilidad activa.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -96,23 +159,38 @@
       <name val="Aptos Narrow"/>
     </font>
     <font>
-      <sz val="11.0"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color theme="0"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+    </font>
     <font/>
+    <font>
+      <sz val="10.0"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -147,6 +225,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF3A7D22"/>
         <bgColor rgb="FF3A7D22"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
       </patternFill>
     </fill>
   </fills>
@@ -200,45 +284,76 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="25">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf quotePrefix="1" borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf quotePrefix="1" borderId="1" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf quotePrefix="1" borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf quotePrefix="1" borderId="1" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" textRotation="45" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" textRotation="45" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" textRotation="45" vertical="center"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -461,7 +576,9 @@
     <col customWidth="1" min="5" max="5" width="15.75"/>
     <col customWidth="1" min="6" max="6" width="10.63"/>
     <col customWidth="1" min="7" max="7" width="12.63"/>
-    <col customWidth="1" min="8" max="26" width="10.63"/>
+    <col customWidth="1" min="8" max="8" width="13.25"/>
+    <col customWidth="1" min="9" max="9" width="41.75"/>
+    <col customWidth="1" min="10" max="26" width="10.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="30.0" customHeight="1">
@@ -471,169 +588,317 @@
     </row>
     <row r="2" ht="40.5" customHeight="1"/>
     <row r="3" ht="86.25" customHeight="1">
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="5">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="4" ht="82.5" customHeight="1">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" ht="82.5" customHeight="1">
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" ht="89.25" customHeight="1">
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
+    </row>
+    <row r="6" ht="38.25" customHeight="1">
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" ht="89.25" customHeight="1">
-      <c r="C5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" ht="38.25" customHeight="1"/>
-    <row r="7" ht="75.0" customHeight="1">
-      <c r="B7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="10" t="s">
+    </row>
+    <row r="7" ht="38.25" customHeight="1"/>
+    <row r="8" ht="75.0" customHeight="1">
+      <c r="B8" s="12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" ht="22.5" customHeight="1">
-      <c r="B8" s="11" t="s">
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="13"/>
-    </row>
-    <row r="9" ht="22.5" customHeight="1">
-      <c r="B9" s="11" t="s">
+      <c r="H8" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-    </row>
-    <row r="10" ht="22.5" customHeight="1">
-      <c r="B10" s="11" t="s">
+      <c r="I8" s="17"/>
+    </row>
+    <row r="9" ht="38.25" customHeight="1">
+      <c r="B9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="14"/>
-    </row>
-    <row r="11" ht="22.5" customHeight="1">
-      <c r="B11" s="11" t="s">
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="3"/>
-    </row>
-    <row r="12" ht="22.5" customHeight="1">
-      <c r="B12" s="11" t="s">
+      <c r="H9" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="13"/>
-    </row>
-    <row r="13" ht="22.5" customHeight="1">
-      <c r="B13" s="11" t="s">
+      <c r="I9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="14"/>
-    </row>
-    <row r="14" ht="22.5" customHeight="1">
-      <c r="B14" s="11" t="s">
+    </row>
+    <row r="10" ht="38.25" customHeight="1">
+      <c r="B10" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-    </row>
-    <row r="15" ht="22.5" customHeight="1">
-      <c r="B15" s="11" t="s">
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" ht="23.25" customHeight="1">
-      <c r="B16" s="11" t="s">
+      <c r="H10" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="13"/>
-    </row>
-    <row r="17" ht="23.25" customHeight="1">
-      <c r="B17" s="11" t="s">
+    </row>
+    <row r="11" ht="38.25" customHeight="1">
+      <c r="B11" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" ht="38.25" customHeight="1">
+      <c r="B12" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" ht="38.25" customHeight="1">
+      <c r="B13" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" ht="38.25" customHeight="1">
+      <c r="B14" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" ht="38.25" customHeight="1">
+      <c r="B15" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="22"/>
+    </row>
+    <row r="16" ht="38.25" customHeight="1">
+      <c r="B16" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" ht="38.25" customHeight="1">
+      <c r="B17" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" ht="38.25" customHeight="1">
+      <c r="B18" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" ht="38.25" customHeight="1">
+      <c r="B19" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" ht="38.25" customHeight="1">
+      <c r="B20" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I20" s="22"/>
+    </row>
+    <row r="21" ht="38.25" customHeight="1">
+      <c r="B21" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" ht="38.25" customHeight="1">
+      <c r="B22" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" s="21" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="23" ht="14.25" customHeight="1"/>
     <row r="24" ht="14.25" customHeight="1"/>
     <row r="25" ht="14.25" customHeight="1"/>
@@ -1599,35 +1864,31 @@
     <row r="985" ht="14.25" customHeight="1"/>
     <row r="986" ht="14.25" customHeight="1"/>
     <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
-    <row r="989" ht="14.25" customHeight="1"/>
-    <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="$B$7:$H$17"/>
-  <mergeCells count="12">
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="B7:F7"/>
+  <autoFilter ref="$B$8:$H$19"/>
+  <mergeCells count="16">
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="B9:F9"/>
     <mergeCell ref="B10:F10"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B13:F13"/>
+    <mergeCell ref="C1:H1"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="B15:F15"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B22:F22"/>
   </mergeCells>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G9:H22">
+      <formula1>"LOW,MEDIUM,HIGH"</formula1>
+    </dataValidation>
+  </dataValidations>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>

</xml_diff>